<commit_message>
feat: remove unused analysis
</commit_message>
<xml_diff>
--- a/tables/table_lethality_rates_2019_2021.xlsx
+++ b/tables/table_lethality_rates_2019_2021.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -661,29 +661,29 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Lethality_Public_Tx</t>
+          <t>Lethality_uti_tx</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11.07253060203237</v>
+        <v>-0.3431171880430295</v>
       </c>
       <c r="D8" t="n">
-        <v>9.555361027960419</v>
+        <v>-2.142180710707942</v>
       </c>
       <c r="E8" t="n">
-        <v>12.61071059033594</v>
+        <v>1.489021152578096</v>
       </c>
       <c r="F8" t="n">
-        <v>10134</v>
+        <v>39867</v>
       </c>
       <c r="G8" t="n">
-        <v>12417</v>
+        <v>39901</v>
       </c>
       <c r="H8" t="n">
-        <v>12450</v>
+        <v>39592</v>
       </c>
       <c r="I8" t="n">
-        <v>22.85375962107756</v>
+        <v>-0.6897935635989666</v>
       </c>
     </row>
     <row r="9">
@@ -692,29 +692,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lethality_Private_Tx</t>
+          <t>Lethality_uti_S_Tx</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>30.69506950265055</v>
+        <v>8.70574001467217</v>
       </c>
       <c r="D9" t="n">
-        <v>22.98082556106369</v>
+        <v>4.187997486319572</v>
       </c>
       <c r="E9" t="n">
-        <v>38.89320643583847</v>
+        <v>13.41937840478338</v>
       </c>
       <c r="F9" t="n">
-        <v>3780</v>
+        <v>34092</v>
       </c>
       <c r="G9" t="n">
-        <v>5348</v>
+        <v>34053</v>
       </c>
       <c r="H9" t="n">
-        <v>6420</v>
+        <v>40388</v>
       </c>
       <c r="I9" t="n">
-        <v>69.84126984126983</v>
+        <v>18.46767570104423</v>
       </c>
     </row>
     <row r="10">
@@ -723,29 +723,29 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lethality_ONG_Tx</t>
+          <t>Lethality_uti_N_Tx</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>19.94943903295248</v>
+        <v>-1.352338033009881</v>
       </c>
       <c r="D10" t="n">
-        <v>18.13513926443264</v>
+        <v>-8.693756849846334</v>
       </c>
       <c r="E10" t="n">
-        <v>21.79160251476324</v>
+        <v>6.579362766577401</v>
       </c>
       <c r="F10" t="n">
-        <v>8225</v>
+        <v>51552</v>
       </c>
       <c r="G10" t="n">
-        <v>10214</v>
+        <v>56526</v>
       </c>
       <c r="H10" t="n">
-        <v>11806</v>
+        <v>49989</v>
       </c>
       <c r="I10" t="n">
-        <v>43.53799392097265</v>
+        <v>-3.031890130353818</v>
       </c>
     </row>
     <row r="11">
@@ -754,29 +754,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lethality_uti_tx</t>
+          <t>Lethality_uti_NE_Tx</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.3431171880430295</v>
+        <v>-1.352338033009881</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.142180710707942</v>
+        <v>-8.693756849846334</v>
       </c>
       <c r="E11" t="n">
-        <v>1.489021152578096</v>
+        <v>6.579362766577401</v>
       </c>
       <c r="F11" t="n">
-        <v>39867</v>
+        <v>51552</v>
       </c>
       <c r="G11" t="n">
-        <v>39901</v>
+        <v>56526</v>
       </c>
       <c r="H11" t="n">
-        <v>39592</v>
+        <v>49989</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.6897935635989666</v>
+        <v>-3.031890130353818</v>
       </c>
     </row>
     <row r="12">
@@ -785,29 +785,29 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Lethality_uti_S_Tx</t>
+          <t>Lethality_uti_SE_Tx</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8.70574001467217</v>
+        <v>0.09068439544728246</v>
       </c>
       <c r="D12" t="n">
-        <v>4.187997486319572</v>
+        <v>-2.574103687616813</v>
       </c>
       <c r="E12" t="n">
-        <v>13.41937840478338</v>
+        <v>2.828359624500498</v>
       </c>
       <c r="F12" t="n">
-        <v>34092</v>
+        <v>37389</v>
       </c>
       <c r="G12" t="n">
-        <v>34053</v>
+        <v>36724</v>
       </c>
       <c r="H12" t="n">
-        <v>40388</v>
+        <v>37431</v>
       </c>
       <c r="I12" t="n">
-        <v>18.46767570104423</v>
+        <v>0.1123325042124689</v>
       </c>
     </row>
     <row r="13">
@@ -816,29 +816,29 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Lethality_uti_N_Tx</t>
+          <t>Lethality_uti_CO_Tx</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-1.352338033009881</v>
+        <v>-3.21181878395681</v>
       </c>
       <c r="D13" t="n">
-        <v>-8.693756849846334</v>
+        <v>-8.565486054774496</v>
       </c>
       <c r="E13" t="n">
-        <v>6.579362766577401</v>
+        <v>2.455316038772337</v>
       </c>
       <c r="F13" t="n">
-        <v>51552</v>
+        <v>42259</v>
       </c>
       <c r="G13" t="n">
-        <v>56526</v>
+        <v>42918</v>
       </c>
       <c r="H13" t="n">
-        <v>49989</v>
+        <v>39330</v>
       </c>
       <c r="I13" t="n">
-        <v>-3.031890130353818</v>
+        <v>-6.931067938190681</v>
       </c>
     </row>
     <row r="14">
@@ -847,29 +847,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Lethality_uti_NE_Tx</t>
+          <t>Lethality_non_uti_Tx</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-1.352338033009881</v>
+        <v>14.9414357382152</v>
       </c>
       <c r="D14" t="n">
-        <v>-8.693756849846334</v>
+        <v>13.54164374982032</v>
       </c>
       <c r="E14" t="n">
-        <v>6.579362766577401</v>
+        <v>16.35848498611474</v>
       </c>
       <c r="F14" t="n">
-        <v>51552</v>
+        <v>6535</v>
       </c>
       <c r="G14" t="n">
-        <v>56526</v>
+        <v>7843</v>
       </c>
       <c r="H14" t="n">
-        <v>49989</v>
+        <v>8607</v>
       </c>
       <c r="I14" t="n">
-        <v>-3.031890130353818</v>
+        <v>31.7061973986228</v>
       </c>
     </row>
     <row r="15">
@@ -878,29 +878,29 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lethality_uti_SE_Tx</t>
+          <t>Lethality_non_uti_S_Tx</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.09068439544728246</v>
+        <v>30.23212302935951</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.574103687616813</v>
+        <v>26.39844905537223</v>
       </c>
       <c r="E15" t="n">
-        <v>2.828359624500498</v>
+        <v>34.18207260837727</v>
       </c>
       <c r="F15" t="n">
-        <v>37389</v>
+        <v>4698</v>
       </c>
       <c r="G15" t="n">
-        <v>36724</v>
+        <v>6038</v>
       </c>
       <c r="H15" t="n">
-        <v>37431</v>
+        <v>7973</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1123325042124689</v>
+        <v>69.71051511281397</v>
       </c>
     </row>
     <row r="16">
@@ -909,29 +909,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Lethality_uti_CO_Tx</t>
+          <t>Lethality_non_uti_N_Tx</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-3.21181878395681</v>
+        <v>9.843325733999686</v>
       </c>
       <c r="D16" t="n">
-        <v>-8.565486054774496</v>
+        <v>4.750020257837484</v>
       </c>
       <c r="E16" t="n">
-        <v>2.455316038772337</v>
+        <v>15.18428520211006</v>
       </c>
       <c r="F16" t="n">
-        <v>42259</v>
+        <v>5915</v>
       </c>
       <c r="G16" t="n">
-        <v>42918</v>
+        <v>6841</v>
       </c>
       <c r="H16" t="n">
-        <v>39330</v>
+        <v>7104</v>
       </c>
       <c r="I16" t="n">
-        <v>-6.931067938190681</v>
+        <v>20.10143702451395</v>
       </c>
     </row>
     <row r="17">
@@ -940,29 +940,29 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Lethality_uti_Public_Tx</t>
+          <t>Lethality_non_uti_NE_Tx</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-1.450071547360365</v>
+        <v>9.843325733999686</v>
       </c>
       <c r="D17" t="n">
-        <v>-4.24990009647761</v>
+        <v>4.750020257837484</v>
       </c>
       <c r="E17" t="n">
-        <v>1.431626784789497</v>
+        <v>15.18428520211006</v>
       </c>
       <c r="F17" t="n">
-        <v>41213</v>
+        <v>5915</v>
       </c>
       <c r="G17" t="n">
-        <v>41644</v>
+        <v>6841</v>
       </c>
       <c r="H17" t="n">
-        <v>40104</v>
+        <v>7104</v>
       </c>
       <c r="I17" t="n">
-        <v>-2.690898502899571</v>
+        <v>20.10143702451395</v>
       </c>
     </row>
     <row r="18">
@@ -971,29 +971,29 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lethality_uti_Private_Tx</t>
+          <t>Lethality_non_uti_SE_Tx</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>12.06432647132074</v>
+        <v>13.53710191105546</v>
       </c>
       <c r="D18" t="n">
-        <v>4.636671399033454</v>
+        <v>11.56836256871352</v>
       </c>
       <c r="E18" t="n">
-        <v>20.01923512626913</v>
+        <v>15.54058169870687</v>
       </c>
       <c r="F18" t="n">
-        <v>33585</v>
+        <v>8322</v>
       </c>
       <c r="G18" t="n">
-        <v>37495</v>
+        <v>9707</v>
       </c>
       <c r="H18" t="n">
-        <v>42235</v>
+        <v>10713</v>
       </c>
       <c r="I18" t="n">
-        <v>25.7555456304898</v>
+        <v>28.73107426099495</v>
       </c>
     </row>
     <row r="19">
@@ -1002,214 +1002,28 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Lethality_uti_ONG_Tx</t>
+          <t>Lethality_non_uti_CO_Tx</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-1.299332684999344</v>
+        <v>17.65726333918107</v>
       </c>
       <c r="D19" t="n">
-        <v>-3.785678904023693</v>
+        <v>11.64161622293005</v>
       </c>
       <c r="E19" t="n">
-        <v>1.251265065922125</v>
+        <v>23.99705490489075</v>
       </c>
       <c r="F19" t="n">
-        <v>40155</v>
+        <v>5267</v>
       </c>
       <c r="G19" t="n">
-        <v>38565</v>
+        <v>5364</v>
       </c>
       <c r="H19" t="n">
-        <v>39176</v>
+        <v>7405</v>
       </c>
       <c r="I19" t="n">
-        <v>-2.438052546382767</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Lethality_non_uti_Tx</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>14.9414357382152</v>
-      </c>
-      <c r="D20" t="n">
-        <v>13.54164374982032</v>
-      </c>
-      <c r="E20" t="n">
-        <v>16.35848498611474</v>
-      </c>
-      <c r="F20" t="n">
-        <v>6535</v>
-      </c>
-      <c r="G20" t="n">
-        <v>7843</v>
-      </c>
-      <c r="H20" t="n">
-        <v>8607</v>
-      </c>
-      <c r="I20" t="n">
-        <v>31.7061973986228</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Lethality_non_uti_S_Tx</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>30.23212302935951</v>
-      </c>
-      <c r="D21" t="n">
-        <v>26.39844905537223</v>
-      </c>
-      <c r="E21" t="n">
-        <v>34.18207260837727</v>
-      </c>
-      <c r="F21" t="n">
-        <v>4698</v>
-      </c>
-      <c r="G21" t="n">
-        <v>6038</v>
-      </c>
-      <c r="H21" t="n">
-        <v>7973</v>
-      </c>
-      <c r="I21" t="n">
-        <v>69.71051511281397</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Lethality_non_uti_N_Tx</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>9.843325733999686</v>
-      </c>
-      <c r="D22" t="n">
-        <v>4.750020257837484</v>
-      </c>
-      <c r="E22" t="n">
-        <v>15.18428520211006</v>
-      </c>
-      <c r="F22" t="n">
-        <v>5915</v>
-      </c>
-      <c r="G22" t="n">
-        <v>6841</v>
-      </c>
-      <c r="H22" t="n">
-        <v>7104</v>
-      </c>
-      <c r="I22" t="n">
-        <v>20.10143702451395</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Lethality_non_uti_NE_Tx</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>9.843325733999686</v>
-      </c>
-      <c r="D23" t="n">
-        <v>4.750020257837484</v>
-      </c>
-      <c r="E23" t="n">
-        <v>15.18428520211006</v>
-      </c>
-      <c r="F23" t="n">
-        <v>5915</v>
-      </c>
-      <c r="G23" t="n">
-        <v>6841</v>
-      </c>
-      <c r="H23" t="n">
-        <v>7104</v>
-      </c>
-      <c r="I23" t="n">
-        <v>20.10143702451395</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Lethality_non_uti_SE_Tx</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>13.53710191105546</v>
-      </c>
-      <c r="D24" t="n">
-        <v>11.56836256871352</v>
-      </c>
-      <c r="E24" t="n">
-        <v>15.54058169870687</v>
-      </c>
-      <c r="F24" t="n">
-        <v>8322</v>
-      </c>
-      <c r="G24" t="n">
-        <v>9707</v>
-      </c>
-      <c r="H24" t="n">
-        <v>10713</v>
-      </c>
-      <c r="I24" t="n">
-        <v>28.73107426099495</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Lethality_non_uti_CO_Tx</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>17.65726333918107</v>
-      </c>
-      <c r="D25" t="n">
-        <v>11.64161622293005</v>
-      </c>
-      <c r="E25" t="n">
-        <v>23.99705490489075</v>
-      </c>
-      <c r="F25" t="n">
-        <v>5267</v>
-      </c>
-      <c r="G25" t="n">
-        <v>5364</v>
-      </c>
-      <c r="H25" t="n">
-        <v>7405</v>
-      </c>
-      <c r="I25" t="n">
         <v>40.59236757167267</v>
       </c>
     </row>

</xml_diff>